<commit_message>
Editing and streamlining of source scripts for running of individual model scripts (for all years).
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v3_test.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v3_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{37DBDE95-57E7-4A54-8D15-5AB9A9FDBC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0934D46-BB28-48F9-A149-83BF6B7F2AFB}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{37DBDE95-57E7-4A54-8D15-5AB9A9FDBC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ECDDC67-DCB3-4B4A-B6B4-EAC43F14786E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="4" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="5" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -3006,7 +3006,7 @@
   </sheetPr>
   <dimension ref="B2:I8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3218,8 +3218,8 @@
   </sheetPr>
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:I4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>